<commit_message>
GU-regrsn cases code change+template update+ADTJira prop file(usrname)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Bug.xlsx
+++ b/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Bug.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.gurulingaiah\Automation_GIT\master\src\test\resources\testdata\DataLoader\GenericUploader\ADTJira\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.gurulingaiah\Automation_GIT_NEW\master\src\test\resources\testdata\DataLoader\GenericUploader\ADTJira\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E633D924-24FB-45E4-B945-D9A51ACFBB2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41AFAAA-51C3-4071-BB43-7E3D0A2B21A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="680" activeTab="2" xr2:uid="{4ADEDBBA-C616-478B-B7B7-DF7FEDCE3438}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="838">
   <si>
     <t>Title</t>
   </si>
@@ -2582,13 +2582,16 @@
     <t>BOM</t>
   </si>
   <si>
-    <t>BOM-125493</t>
-  </si>
-  <si>
-    <t>Bug_AutomationData</t>
-  </si>
-  <si>
     <t>2021-11-03T06:36:53Z</t>
+  </si>
+  <si>
+    <t>BOM-125890</t>
+  </si>
+  <si>
+    <t>BUG_AUTOMATION</t>
+  </si>
+  <si>
+    <t>Bug_AutomationData_02</t>
   </si>
 </sst>
 </file>
@@ -10130,7 +10133,7 @@
   <dimension ref="A1:BH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10370,19 +10373,22 @@
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C2" t="s">
-        <v>835</v>
+        <v>837</v>
+      </c>
+      <c r="D2" t="s">
+        <v>836</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>833</v>
       </c>
       <c r="L2" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="M2" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
   </sheetData>
@@ -10719,12 +10725,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10907,15 +10910,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F359188-8654-4AC8-AEDD-04D6FE3DA0A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87BCECA1-7A17-4605-AE73-73B4F527C894}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="acee2d6b-dd79-4fb3-8fb4-89e5568edfef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bc0735e1-1781-4e64-a3a6-cf1bacd21285"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10940,18 +10955,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87BCECA1-7A17-4605-AE73-73B4F527C894}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F359188-8654-4AC8-AEDD-04D6FE3DA0A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="acee2d6b-dd79-4fb3-8fb4-89e5568edfef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bc0735e1-1781-4e64-a3a6-cf1bacd21285"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>